<commit_message>
fixed odd rows in ID and WA data
</commit_message>
<xml_diff>
--- a/data/raw/USFWS_bull_trout_SSA_data_ID_v2.xlsx
+++ b/data/raw/USFWS_bull_trout_SSA_data_ID_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheuerl/Documents/GitHub/bulltrout/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913EEE2F-27EC-9046-A07A-8582A764B87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4012F5C-C6C9-D546-AC2D-12280F1DF331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="28800" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ID_data" sheetId="1" r:id="rId1"/>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB1341"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A935" workbookViewId="0">
+      <selection activeCell="A940" sqref="A940:D941"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25482,7 +25482,7 @@
         <v>62</v>
       </c>
       <c r="D941" s="12" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E941" s="12" t="s">
         <v>7</v>
@@ -35905,17 +35905,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="I1327:J1327"/>
-    <mergeCell ref="I1328:J1328"/>
-    <mergeCell ref="I1330:J1330"/>
-    <mergeCell ref="I1331:J1331"/>
-    <mergeCell ref="I1332:J1332"/>
     <mergeCell ref="I1339:J1339"/>
     <mergeCell ref="I1340:J1340"/>
     <mergeCell ref="I1334:J1334"/>
     <mergeCell ref="I1335:J1335"/>
     <mergeCell ref="I1336:J1336"/>
     <mergeCell ref="I1338:J1338"/>
+    <mergeCell ref="I1327:J1327"/>
+    <mergeCell ref="I1328:J1328"/>
+    <mergeCell ref="I1330:J1330"/>
+    <mergeCell ref="I1331:J1331"/>
+    <mergeCell ref="I1332:J1332"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -36693,18 +36693,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36727,14 +36727,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFAABD42-B977-47B6-983A-D015976BBDFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{407EB793-7EF8-47E0-9BDA-5F3E759227C3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -36749,4 +36741,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFAABD42-B977-47B6-983A-D015976BBDFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>